<commit_message>
update monitoring trend lines in price functions excel file
</commit_message>
<xml_diff>
--- a/calculator/price-functions.xlsx
+++ b/calculator/price-functions.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uzhne/project-extras/imarket/expert/requirements/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uzhne/project-extras/imarket/expert/src/calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="940" yWindow="460" windowWidth="37460" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="940" yWindow="460" windowWidth="37460" windowHeight="21140" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="examination" sheetId="4" r:id="rId1"/>
@@ -361,11 +361,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2089641728"/>
-        <c:axId val="2097193312"/>
+        <c:axId val="-2089860576"/>
+        <c:axId val="-2096036800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2089641728"/>
+        <c:axId val="-2089860576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -422,12 +422,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2097193312"/>
+        <c:crossAx val="-2096036800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2097193312"/>
+        <c:axId val="-2096036800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -484,7 +484,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2089641728"/>
+        <c:crossAx val="-2089860576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1081,11 +1081,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2092354272"/>
-        <c:axId val="-2119041264"/>
+        <c:axId val="-2062933648"/>
+        <c:axId val="-2063203088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2092354272"/>
+        <c:axId val="-2062933648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1142,12 +1142,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2119041264"/>
+        <c:crossAx val="-2063203088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2119041264"/>
+        <c:axId val="-2063203088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1204,7 +1204,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2092354272"/>
+        <c:crossAx val="-2062933648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1267,37 +1267,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1340,11 +1309,191 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'monitoring &amp; oversight'!$A$2:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12000.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14000.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18000.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20000.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30000.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40000.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50000.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>60000.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>70000.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80000.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90000.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>110000.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>120000.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>200000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'monitoring &amp; oversight'!$B$2:$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0" formatCode="0.00">
+                  <c:v>120.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72.27</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00">
+                  <c:v>43.42</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00">
+                  <c:v>22.89</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00">
+                  <c:v>18.53</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00">
+                  <c:v>15.56</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00">
+                  <c:v>13.75</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.00">
+                  <c:v>12.28</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00">
+                  <c:v>11.1</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00">
+                  <c:v>10.14</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.00">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.00">
+                  <c:v>8.1</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="0.00">
+                  <c:v>7.62</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="0.00">
+                  <c:v>7.16</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="0.00">
+                  <c:v>6.73</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="0.00">
+                  <c:v>6.32</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="0.00">
+                  <c:v>5.93</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="0.00">
+                  <c:v>5.56</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="0.00">
+                  <c:v>5.22</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="0.00">
+                  <c:v>4.9</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="0.00">
+                  <c:v>4.6</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="0.00">
+                  <c:v>3.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
           <c:trendline>
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
                 <a:prstDash val="sysDot"/>
               </a:ln>
@@ -1356,8 +1505,338 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.0334667716042604"/>
-                  <c:y val="-0.0856077736555066"/>
+                  <c:x val="0.101160438692014"/>
+                  <c:y val="-0.693759647478522"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="0.000000000000000000000000000000" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'monitoring &amp; oversight'!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12000.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14000.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18000.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'monitoring &amp; oversight'!$B$2:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0" formatCode="0.00">
+                  <c:v>120.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72.27</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00">
+                  <c:v>43.42</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00">
+                  <c:v>22.89</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00">
+                  <c:v>18.53</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00">
+                  <c:v>15.56</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00">
+                  <c:v>13.75</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.00">
+                  <c:v>12.28</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00">
+                  <c:v>11.1</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00">
+                  <c:v>10.14</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.00">
+                  <c:v>9.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>3</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:forward val="50000.0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.116154166275927"/>
+                  <c:y val="-0.0901027819729151"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="0.000000000000000000000000000000" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'monitoring &amp; oversight'!$A$13:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>30000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70000.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90000.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>110000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>120000.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>200000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'monitoring &amp; oversight'!$B$13:$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>8.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.62</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.73</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.93</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.56</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.22</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.120496556396524"/>
+                  <c:y val="-0.0493469763407814"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1392,150 +1871,30 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'monitoring &amp; oversight'!$A$2:$A$23</c:f>
+              <c:f>'monitoring &amp; oversight'!$A$12:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>500.0</c:v>
+                  <c:v>20000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1000.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2500.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5000.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7500.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10000.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12000.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>14000.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>16000.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>18000.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>20000.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>30000.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>40000.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>50000.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>60000.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>70000.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>80000.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>90000.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>100000.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>110000.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>120000.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>200000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'monitoring &amp; oversight'!$B$2:$B$23</c:f>
+              <c:f>'monitoring &amp; oversight'!$B$12:$B$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
-                <c:pt idx="0" formatCode="0.00">
-                  <c:v>120.0</c:v>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>9.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>72.27</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="0.00">
-                  <c:v>43.42</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="0.00">
-                  <c:v>22.89</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="0.00">
-                  <c:v>18.53</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="0.00">
-                  <c:v>15.56</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="0.00">
-                  <c:v>13.75</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="0.00">
-                  <c:v>12.28</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="0.00">
-                  <c:v>11.1</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="0.00">
-                  <c:v>10.14</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="0.00">
-                  <c:v>9.4</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="0.00">
                   <c:v>8.1</c:v>
-                </c:pt>
-                <c:pt idx="12" formatCode="0.00">
-                  <c:v>7.62</c:v>
-                </c:pt>
-                <c:pt idx="13" formatCode="0.00">
-                  <c:v>7.16</c:v>
-                </c:pt>
-                <c:pt idx="14" formatCode="0.00">
-                  <c:v>6.73</c:v>
-                </c:pt>
-                <c:pt idx="15" formatCode="0.00">
-                  <c:v>6.32</c:v>
-                </c:pt>
-                <c:pt idx="16" formatCode="0.00">
-                  <c:v>5.93</c:v>
-                </c:pt>
-                <c:pt idx="17" formatCode="0.00">
-                  <c:v>5.56</c:v>
-                </c:pt>
-                <c:pt idx="18" formatCode="0.00">
-                  <c:v>5.22</c:v>
-                </c:pt>
-                <c:pt idx="19" formatCode="0.00">
-                  <c:v>4.9</c:v>
-                </c:pt>
-                <c:pt idx="20" formatCode="0.00">
-                  <c:v>4.6</c:v>
-                </c:pt>
-                <c:pt idx="21" formatCode="0.00">
-                  <c:v>3.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1550,11 +1909,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2145145024"/>
-        <c:axId val="2145148304"/>
+        <c:axId val="-2101759104"/>
+        <c:axId val="-2101586192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2145145024"/>
+        <c:axId val="-2101759104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1611,12 +1970,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2145148304"/>
+        <c:crossAx val="-2101586192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2145148304"/>
+        <c:axId val="-2101586192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1673,7 +2032,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2145145024"/>
+        <c:crossAx val="-2101759104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3760,8 +4119,8 @@
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="173" zoomScaleNormal="173" zoomScalePageLayoutView="173" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="91" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4108,8 +4467,8 @@
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView zoomScale="161" zoomScaleNormal="161" zoomScalePageLayoutView="161" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add inspection calculator price function
</commit_message>
<xml_diff>
--- a/calculator/price-functions.xlsx
+++ b/calculator/price-functions.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="940" yWindow="460" windowWidth="37460" windowHeight="21140" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="940" yWindow="460" windowWidth="28160" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="examination" sheetId="4" r:id="rId1"/>
-    <sheet name="monitoring &amp; oversight" sheetId="1" r:id="rId2"/>
+    <sheet name="inspection" sheetId="5" r:id="rId1"/>
+    <sheet name="examination" sheetId="4" r:id="rId2"/>
+    <sheet name="monitoring &amp; oversight" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
   <si>
     <t>кв.м.</t>
   </si>
@@ -46,12 +47,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -66,10 +79,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -85,6 +101,1179 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.00846531922363208"/>
+                  <c:y val="-0.169612352453048"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>inspection!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>inspection!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0" formatCode="0.00">
+                  <c:v>240.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>145.23</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00">
+                  <c:v>115.57</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00">
+                  <c:v>95.8</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00">
+                  <c:v>80.4</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00">
+                  <c:v>60.62</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>inspection!$A$8:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>20000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60000.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80000.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>90000.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>110000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>inspection!$B$8:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>51.26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41.41</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>34.68</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29.85</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26.16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23.31</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19.38</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16.85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2100972912"/>
+        <c:axId val="-2062340112"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2100972912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2062340112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2062340112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2100972912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>3</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:forward val="5000.0"/>
+            <c:backward val="5000.0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0906599978835451"/>
+                  <c:y val="-0.0898326535304831"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>inspection!$A$9:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>30000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70000.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90000.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>110000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>120000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>inspection!$B$9:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>41.41</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34.68</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29.85</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23.31</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19.38</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16.85</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:forward val="5000.0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.114649662361927"/>
+                  <c:y val="-0.572052724178708"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>inspection!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>inspection!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0" formatCode="0.00">
+                  <c:v>240.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>145.23</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00">
+                  <c:v>115.57</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00">
+                  <c:v>95.8</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00">
+                  <c:v>80.4</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00">
+                  <c:v>60.62</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.109621326776447"/>
+                  <c:y val="-0.0928320712412907"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>inspection!$A$7:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>15000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>inspection!$B$7:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>60.62</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51.26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41.41</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>4</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:forward val="50000.0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0432567592395541"/>
+                  <c:y val="-0.0580285391523154"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>inspection!$A$18:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>120000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>inspection!$B$18:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>15.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.23</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2135781616"/>
+        <c:axId val="-2135029184"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2135781616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2135029184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2135029184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2135781616"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
@@ -533,7 +1722,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
@@ -1253,7 +2442,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
@@ -2201,6 +3390,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3749,7 +5018,1108 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>617096</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>126306</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>820297</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>126306</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>617096</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>157535</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>820297</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>157535</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3818,7 +6188,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4116,11 +6486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="91" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="180" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4134,213 +6503,220 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+      <c r="A2" s="4">
         <v>500</v>
       </c>
-      <c r="B2" s="1">
-        <v>80</v>
+      <c r="B2" s="4">
+        <v>240</v>
       </c>
       <c r="C2" s="1">
         <f>A2*B2</f>
-        <v>40000</v>
+        <v>120000</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="A3" s="4">
         <v>2500</v>
       </c>
-      <c r="B3" s="2">
-        <v>59.7</v>
+      <c r="B3" s="5">
+        <v>145.22999999999999</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:C18" si="0">A3*B3</f>
-        <v>149250</v>
+        <f t="shared" ref="C3:C19" si="0">A3*B3</f>
+        <v>363075</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+      <c r="A4" s="4">
         <v>5000</v>
       </c>
-      <c r="B4" s="1">
-        <v>51.17</v>
+      <c r="B4" s="4">
+        <v>115.57</v>
       </c>
       <c r="C4" s="1">
         <f t="shared" si="0"/>
-        <v>255850</v>
+        <v>577850</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+      <c r="A5" s="4">
         <v>7500</v>
       </c>
-      <c r="B5" s="1">
-        <v>45.24</v>
+      <c r="B5" s="4">
+        <v>95.8</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" si="0"/>
-        <v>339300</v>
+        <v>718500</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+      <c r="A6" s="4">
         <v>10000</v>
       </c>
-      <c r="B6" s="1">
-        <v>40.630000000000003</v>
+      <c r="B6" s="4">
+        <v>80.400000000000006</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="0"/>
-        <v>406300</v>
+        <v>804000</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>20000</v>
-      </c>
-      <c r="B7" s="1">
-        <v>28.21</v>
+      <c r="A7" s="4">
+        <v>15000</v>
+      </c>
+      <c r="B7" s="4">
+        <v>60.62</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" si="0"/>
-        <v>564200</v>
+        <v>909300</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="B8" s="1">
-        <v>20.23</v>
+        <v>51.26</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" si="0"/>
-        <v>606900</v>
+        <v>1025200</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>40000</v>
-      </c>
-      <c r="B9" s="1">
-        <v>16.28</v>
+      <c r="A9" s="3">
+        <v>30000</v>
+      </c>
+      <c r="B9" s="3">
+        <v>41.41</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" si="0"/>
-        <v>651200</v>
+        <v>1242300</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>50000</v>
-      </c>
-      <c r="B10" s="1">
-        <v>13.58</v>
+      <c r="A10" s="3">
+        <v>40000</v>
+      </c>
+      <c r="B10" s="3">
+        <v>34.68</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" si="0"/>
-        <v>679000</v>
+        <v>1387200</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>60000</v>
-      </c>
-      <c r="B11" s="1">
-        <v>11.74</v>
+      <c r="A11" s="3">
+        <v>50000</v>
+      </c>
+      <c r="B11" s="3">
+        <v>29.85</v>
       </c>
       <c r="C11" s="1">
         <f t="shared" si="0"/>
-        <v>704400</v>
+        <v>1492500</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>70000</v>
-      </c>
-      <c r="B12" s="1">
-        <v>10.6</v>
+      <c r="A12" s="3">
+        <v>60000</v>
+      </c>
+      <c r="B12" s="3">
+        <v>26.16</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" si="0"/>
-        <v>742000</v>
+        <v>1569600</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>80000</v>
-      </c>
-      <c r="B13" s="1">
-        <v>10.029999999999999</v>
+      <c r="A13" s="3">
+        <v>70000</v>
+      </c>
+      <c r="B13" s="3">
+        <v>23.31</v>
       </c>
       <c r="C13" s="1">
         <f t="shared" si="0"/>
-        <v>802400</v>
+        <v>1631700</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>90000</v>
-      </c>
-      <c r="B14" s="1">
-        <v>9.83</v>
+      <c r="A14" s="3">
+        <v>80000</v>
+      </c>
+      <c r="B14" s="3">
+        <v>21.1</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" si="0"/>
-        <v>884700</v>
+        <v>1688000</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>100000</v>
-      </c>
-      <c r="B15" s="1">
-        <v>9.76</v>
+      <c r="A15" s="3">
+        <v>90000</v>
+      </c>
+      <c r="B15" s="3">
+        <v>19.38</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" si="0"/>
-        <v>976000</v>
+        <v>1744200</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>110000</v>
-      </c>
-      <c r="B16" s="1">
-        <v>9.65</v>
+      <c r="A16" s="3">
+        <v>100000</v>
+      </c>
+      <c r="B16" s="3">
+        <v>18</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" si="0"/>
-        <v>1061500</v>
+        <v>1800000</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>120000</v>
-      </c>
-      <c r="B17" s="1">
-        <v>9.4600000000000009</v>
+      <c r="A17" s="3">
+        <v>110000</v>
+      </c>
+      <c r="B17" s="3">
+        <v>16.850000000000001</v>
       </c>
       <c r="C17" s="1">
         <f t="shared" si="0"/>
-        <v>1135200</v>
+        <v>1853500.0000000002</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>200000</v>
-      </c>
-      <c r="B18" s="1">
-        <v>7.73</v>
+      <c r="A18" s="3">
+        <v>120000</v>
+      </c>
+      <c r="B18" s="3">
+        <v>15.9</v>
       </c>
       <c r="C18" s="1">
         <f t="shared" si="0"/>
-        <v>1546000</v>
+        <v>1908000</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="A19" s="1">
+        <v>200000</v>
+      </c>
+      <c r="B19" s="1">
+        <v>13.23</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="0"/>
+        <v>2646000</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
@@ -4464,11 +6840,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
+  <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="91" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4486,6 +6862,354 @@
         <v>500</v>
       </c>
       <c r="B2" s="1">
+        <v>80</v>
+      </c>
+      <c r="C2" s="1">
+        <f>A2*B2</f>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>2500</v>
+      </c>
+      <c r="B3" s="2">
+        <v>59.7</v>
+      </c>
+      <c r="C3" s="1">
+        <f t="shared" ref="C3:C18" si="0">A3*B3</f>
+        <v>149250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>5000</v>
+      </c>
+      <c r="B4" s="1">
+        <v>51.17</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" si="0"/>
+        <v>255850</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>7500</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45.24</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" si="0"/>
+        <v>339300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>10000</v>
+      </c>
+      <c r="B6" s="1">
+        <v>40.630000000000003</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" si="0"/>
+        <v>406300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>20000</v>
+      </c>
+      <c r="B7" s="1">
+        <v>28.21</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="0"/>
+        <v>564200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>30000</v>
+      </c>
+      <c r="B8" s="1">
+        <v>20.23</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
+        <v>606900</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>40000</v>
+      </c>
+      <c r="B9" s="1">
+        <v>16.28</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="0"/>
+        <v>651200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>50000</v>
+      </c>
+      <c r="B10" s="1">
+        <v>13.58</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="0"/>
+        <v>679000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>60000</v>
+      </c>
+      <c r="B11" s="1">
+        <v>11.74</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" si="0"/>
+        <v>704400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>70000</v>
+      </c>
+      <c r="B12" s="1">
+        <v>10.6</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" si="0"/>
+        <v>742000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>80000</v>
+      </c>
+      <c r="B13" s="1">
+        <v>10.029999999999999</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" si="0"/>
+        <v>802400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>90000</v>
+      </c>
+      <c r="B14" s="1">
+        <v>9.83</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" si="0"/>
+        <v>884700</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>100000</v>
+      </c>
+      <c r="B15" s="1">
+        <v>9.76</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" si="0"/>
+        <v>976000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>110000</v>
+      </c>
+      <c r="B16" s="1">
+        <v>9.65</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" si="0"/>
+        <v>1061500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>120000</v>
+      </c>
+      <c r="B17" s="1">
+        <v>9.4600000000000009</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="0"/>
+        <v>1135200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>200000</v>
+      </c>
+      <c r="B18" s="1">
+        <v>7.73</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="0"/>
+        <v>1546000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C40" s="1"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C43" s="1"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C44" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:C44"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>500</v>
+      </c>
+      <c r="B2" s="1">
         <v>120</v>
       </c>
       <c r="C2" s="1">

</xml_diff>